<commit_message>
API for verify account and resend otp added
</commit_message>
<xml_diff>
--- a/API's/API endpoint.xlsx
+++ b/API's/API endpoint.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>API endpoints</t>
   </si>
@@ -119,6 +119,18 @@
     "email": "Pokhara",
     "phoneNumber": "9815158175"
 }</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/kinMel/verify-account?email=suman.yhhits@gmail.com&amp;otp=927583</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>OTP verified.Now you can login</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/kinMel/regenerate-otp?email=dssuman222@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -163,12 +175,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -471,16 +489,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="1" max="1" width="74.88671875" customWidth="1"/>
+    <col min="2" max="2" width="48.88671875" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="91.33203125" customWidth="1"/>
   </cols>
@@ -525,8 +543,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
@@ -539,9 +557,37 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="A6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>